<commit_message>
cleanup mircostepping with 16steps -> TODO experiment with decay, get 32steps?
</commit_message>
<xml_diff>
--- a/motor.xlsx
+++ b/motor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://smobvba-my.sharepoint.com/personal/jorik_wittevrongel_smo_be/Documents/Bureaublad/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorik Wittevrongel\LocalProjects\901-PersonalGit\DRV8823_Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{42DC5812-33D8-402B-946E-B988AECA0EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27A8C316-DDAB-4883-9281-A7F22E849990}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928B9DAD-3B5E-4FE3-ADFF-80A813CB998F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{889D07B9-8686-4B9C-91D8-34E3E65293CC}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="55">
   <si>
     <t>–5%</t>
   </si>
@@ -196,6 +195,12 @@
   </si>
   <si>
     <t>hex</t>
+  </si>
+  <si>
+    <t>cleanup hex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add 0x </t>
   </si>
 </sst>
 </file>
@@ -632,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14006E83-6050-44C0-8466-4E9A6B1E0657}">
-  <dimension ref="A1:AD129"/>
+  <dimension ref="A1:AE129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q129"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,9 +648,11 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.7109375" customWidth="1"/>
     <col min="16" max="16" width="18.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -683,23 +690,29 @@
       <c r="Q1" t="s">
         <v>52</v>
       </c>
-      <c r="T1" t="s">
+      <c r="R1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" t="s">
         <v>46</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>47</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>48</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -747,38 +760,46 @@
         <f>DEC2HEX(O2,4)</f>
         <v>001D</v>
       </c>
-      <c r="T2" s="10">
-        <v>1</v>
-      </c>
-      <c r="U2" s="1">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="R2" t="str">
+        <f>Q2</f>
+        <v>001D</v>
+      </c>
+      <c r="S2" t="str">
+        <f>"0x"&amp;R2</f>
+        <v>0x001D</v>
+      </c>
+      <c r="U2" s="10">
+        <v>1</v>
+      </c>
+      <c r="V2" s="1">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -826,29 +847,29 @@
         <f t="shared" ref="Q3:Q66" si="1">DEC2HEX(O3,4)</f>
         <v>001D</v>
       </c>
-      <c r="T3" s="10">
-        <v>1</v>
-      </c>
-      <c r="U3" s="1">
+      <c r="U3" s="10">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
         <v>0.05</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>3</v>
       </c>
-      <c r="X3">
-        <v>0</v>
-      </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AA3" s="18">
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="18">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -896,29 +917,37 @@
         <f t="shared" si="1"/>
         <v>0019</v>
       </c>
-      <c r="T4" s="8">
-        <v>1</v>
-      </c>
-      <c r="U4" s="1">
+      <c r="R4" t="str">
+        <f t="shared" ref="R4" si="2">Q4</f>
+        <v>0019</v>
+      </c>
+      <c r="S4" t="str">
+        <f t="shared" ref="S4" si="3">"0x"&amp;R4</f>
+        <v>0x0019</v>
+      </c>
+      <c r="U4" s="8">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
         <v>0.1</v>
       </c>
-      <c r="V4">
+      <c r="W4">
         <v>6</v>
       </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
       <c r="Y4">
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="17">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -966,29 +995,29 @@
         <f t="shared" si="1"/>
         <v>0059</v>
       </c>
-      <c r="T5" s="8">
+      <c r="U5" s="8">
         <v>0.99</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>0.15</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>8</v>
       </c>
-      <c r="X5">
-        <v>0</v>
-      </c>
       <c r="Y5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="16">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="16">
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1036,29 +1065,37 @@
         <f t="shared" si="1"/>
         <v>0059</v>
       </c>
-      <c r="T6" s="8">
+      <c r="R6" t="str">
+        <f t="shared" ref="R6" si="4">Q6</f>
+        <v>0059</v>
+      </c>
+      <c r="S6" t="str">
+        <f t="shared" ref="S6" si="5">"0x"&amp;R6</f>
+        <v>0x0059</v>
+      </c>
+      <c r="U6" s="8">
         <v>0.98</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>0.2</v>
       </c>
-      <c r="V6">
+      <c r="W6">
         <v>11</v>
       </c>
-      <c r="X6">
-        <v>0</v>
-      </c>
       <c r="Y6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6">
         <v>1</v>
       </c>
-      <c r="AA6" s="15">
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="15">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1106,29 +1143,29 @@
         <f t="shared" si="1"/>
         <v>0059</v>
       </c>
-      <c r="T7" s="8">
+      <c r="U7" s="8">
         <v>0.97</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>0.24</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <v>14</v>
       </c>
-      <c r="X7">
-        <v>1</v>
-      </c>
       <c r="Y7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <v>0</v>
       </c>
-      <c r="AA7" s="14">
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="14">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1176,29 +1213,37 @@
         <f t="shared" si="1"/>
         <v>0055</v>
       </c>
-      <c r="T8" s="7">
+      <c r="R8" t="str">
+        <f t="shared" ref="R8" si="6">Q8</f>
+        <v>0055</v>
+      </c>
+      <c r="S8" t="str">
+        <f t="shared" ref="S8" si="7">"0x"&amp;R8</f>
+        <v>0x0055</v>
+      </c>
+      <c r="U8" s="7">
         <v>0.96</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>17</v>
       </c>
-      <c r="X8">
-        <v>1</v>
-      </c>
       <c r="Y8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="13">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1246,29 +1291,29 @@
         <f t="shared" si="1"/>
         <v>0155</v>
       </c>
-      <c r="T9" s="7">
+      <c r="U9" s="7">
         <v>0.94</v>
       </c>
-      <c r="U9" s="3">
+      <c r="V9" s="3">
         <v>0.34</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <v>20</v>
       </c>
-      <c r="X9">
-        <v>1</v>
-      </c>
       <c r="Y9">
         <v>1</v>
       </c>
       <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="11">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="11">
         <v>98</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1316,29 +1361,37 @@
         <f t="shared" si="1"/>
         <v>0155</v>
       </c>
-      <c r="T10" s="7">
+      <c r="R10" t="str">
+        <f t="shared" ref="R10" si="8">Q10</f>
+        <v>0155</v>
+      </c>
+      <c r="S10" t="str">
+        <f t="shared" ref="S10" si="9">"0x"&amp;R10</f>
+        <v>0x0155</v>
+      </c>
+      <c r="U10" s="7">
         <v>0.92</v>
       </c>
-      <c r="U10" s="3">
+      <c r="V10" s="3">
         <v>0.38</v>
       </c>
-      <c r="V10">
+      <c r="W10">
         <v>23</v>
       </c>
-      <c r="X10">
-        <v>1</v>
-      </c>
       <c r="Y10">
         <v>1</v>
       </c>
       <c r="Z10">
         <v>1</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AA10">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="12">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1386,17 +1439,17 @@
         <f t="shared" si="1"/>
         <v>0155</v>
       </c>
-      <c r="T11" s="7">
+      <c r="U11" s="7">
         <v>0.9</v>
       </c>
-      <c r="U11" s="3">
+      <c r="V11" s="3">
         <v>0.43</v>
       </c>
-      <c r="V11">
+      <c r="W11">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1437,24 +1490,32 @@
         <v>1</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O75" si="2">C12*POWER(2,11)+D12*POWER(2,10)+E12*POWER(2,9)+F12*POWER(2,8)+G12*POWER(2,7)+H12*POWER(2,6)+I12*POWER(2,5)+J12*POWER(2,4)+K12*POWER(2,3)+L12*POWER(2,2)+M12*POWER(2,1)+N12*POWER(2,0)</f>
+        <f t="shared" ref="O12:O75" si="10">C12*POWER(2,11)+D12*POWER(2,10)+E12*POWER(2,9)+F12*POWER(2,8)+G12*POWER(2,7)+H12*POWER(2,6)+I12*POWER(2,5)+J12*POWER(2,4)+K12*POWER(2,3)+L12*POWER(2,2)+M12*POWER(2,1)+N12*POWER(2,0)</f>
         <v>337</v>
       </c>
       <c r="Q12" t="str">
         <f t="shared" si="1"/>
         <v>0151</v>
       </c>
-      <c r="T12" s="4">
+      <c r="R12" t="str">
+        <f t="shared" ref="R12" si="11">Q12</f>
+        <v>0151</v>
+      </c>
+      <c r="S12" t="str">
+        <f t="shared" ref="S12" si="12">"0x"&amp;R12</f>
+        <v>0x0151</v>
+      </c>
+      <c r="U12" s="4">
         <v>0.88</v>
       </c>
-      <c r="U12" s="3">
+      <c r="V12" s="3">
         <v>0.47</v>
       </c>
-      <c r="V12">
+      <c r="W12">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1495,24 +1556,24 @@
         <v>1</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>593</v>
       </c>
       <c r="Q13" t="str">
         <f t="shared" si="1"/>
         <v>0251</v>
       </c>
-      <c r="T13" s="4">
+      <c r="U13" s="4">
         <v>0.86</v>
       </c>
-      <c r="U13" s="6">
+      <c r="V13" s="6">
         <v>0.51</v>
       </c>
-      <c r="V13">
+      <c r="W13">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1553,24 +1614,32 @@
         <v>1</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>593</v>
       </c>
       <c r="Q14" t="str">
         <f t="shared" si="1"/>
         <v>0251</v>
       </c>
-      <c r="T14" s="4">
+      <c r="R14" t="str">
+        <f t="shared" ref="R14" si="13">Q14</f>
+        <v>0251</v>
+      </c>
+      <c r="S14" t="str">
+        <f t="shared" ref="S14" si="14">"0x"&amp;R14</f>
+        <v>0x0251</v>
+      </c>
+      <c r="U14" s="4">
         <v>0.83</v>
       </c>
-      <c r="U14" s="6">
+      <c r="V14" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1611,24 +1680,24 @@
         <v>1</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>593</v>
       </c>
       <c r="Q15" t="str">
         <f t="shared" si="1"/>
         <v>0251</v>
       </c>
-      <c r="T15" s="4">
+      <c r="U15" s="4">
         <v>0.8</v>
       </c>
-      <c r="U15" s="6">
+      <c r="V15" s="6">
         <v>0.6</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1669,24 +1738,32 @@
         <v>1</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>589</v>
       </c>
       <c r="Q16" t="str">
         <f t="shared" si="1"/>
         <v>024D</v>
       </c>
-      <c r="T16" s="5">
+      <c r="R16" t="str">
+        <f t="shared" ref="R16" si="15">Q16</f>
+        <v>024D</v>
+      </c>
+      <c r="S16" t="str">
+        <f t="shared" ref="S16" si="16">"0x"&amp;R16</f>
+        <v>0x024D</v>
+      </c>
+      <c r="U16" s="5">
         <v>0.77</v>
       </c>
-      <c r="U16" s="6">
+      <c r="V16" s="6">
         <v>0.63</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1727,24 +1804,24 @@
         <v>1</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>845</v>
       </c>
       <c r="Q17" t="str">
         <f t="shared" si="1"/>
         <v>034D</v>
       </c>
-      <c r="T17" s="5">
+      <c r="U17" s="5">
         <v>0.74</v>
       </c>
-      <c r="U17" s="5">
+      <c r="V17" s="5">
         <v>0.67</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1785,24 +1862,32 @@
         <v>1</v>
       </c>
       <c r="O18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>845</v>
       </c>
       <c r="Q18" t="str">
         <f t="shared" si="1"/>
         <v>034D</v>
       </c>
-      <c r="T18" s="5">
-        <v>0.71</v>
+      <c r="R18" t="str">
+        <f t="shared" ref="R18" si="17">Q18</f>
+        <v>034D</v>
+      </c>
+      <c r="S18" t="str">
+        <f t="shared" ref="S18" si="18">"0x"&amp;R18</f>
+        <v>0x034D</v>
       </c>
       <c r="U18" s="5">
         <v>0.71</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="W18">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1843,24 +1928,24 @@
         <v>1</v>
       </c>
       <c r="O19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>845</v>
       </c>
       <c r="Q19" t="str">
         <f t="shared" si="1"/>
         <v>034D</v>
       </c>
-      <c r="T19" s="5">
+      <c r="U19" s="5">
         <v>0.67</v>
       </c>
-      <c r="U19" s="5">
+      <c r="V19" s="5">
         <v>0.74</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1901,24 +1986,32 @@
         <v>1</v>
       </c>
       <c r="O20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>841</v>
       </c>
       <c r="Q20" t="str">
         <f t="shared" si="1"/>
         <v>0349</v>
       </c>
-      <c r="T20" s="6">
+      <c r="R20" t="str">
+        <f t="shared" ref="R20" si="19">Q20</f>
+        <v>0349</v>
+      </c>
+      <c r="S20" t="str">
+        <f t="shared" ref="S20" si="20">"0x"&amp;R20</f>
+        <v>0x0349</v>
+      </c>
+      <c r="U20" s="6">
         <v>0.63</v>
       </c>
-      <c r="U20" s="5">
+      <c r="V20" s="5">
         <v>0.77</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1959,24 +2052,24 @@
         <v>1</v>
       </c>
       <c r="O21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1097</v>
       </c>
       <c r="Q21" t="str">
         <f t="shared" si="1"/>
         <v>0449</v>
       </c>
-      <c r="T21" s="6">
+      <c r="U21" s="6">
         <v>0.6</v>
       </c>
-      <c r="U21" s="4">
+      <c r="V21" s="4">
         <v>0.8</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2017,24 +2110,32 @@
         <v>1</v>
       </c>
       <c r="O22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1097</v>
       </c>
       <c r="Q22" t="str">
         <f t="shared" si="1"/>
         <v>0449</v>
       </c>
-      <c r="T22" s="6">
+      <c r="R22" t="str">
+        <f t="shared" ref="R22" si="21">Q22</f>
+        <v>0449</v>
+      </c>
+      <c r="S22" t="str">
+        <f t="shared" ref="S22" si="22">"0x"&amp;R22</f>
+        <v>0x0449</v>
+      </c>
+      <c r="U22" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U22" s="4">
+      <c r="V22" s="4">
         <v>0.83</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2075,24 +2176,24 @@
         <v>1</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1097</v>
       </c>
       <c r="Q23" t="str">
         <f t="shared" si="1"/>
         <v>0449</v>
       </c>
-      <c r="T23" s="6">
+      <c r="U23" s="6">
         <v>0.51</v>
       </c>
-      <c r="U23" s="4">
+      <c r="V23" s="4">
         <v>0.86</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2133,24 +2234,32 @@
         <v>1</v>
       </c>
       <c r="O24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1093</v>
       </c>
       <c r="Q24" t="str">
         <f t="shared" si="1"/>
         <v>0445</v>
       </c>
-      <c r="T24" s="3">
+      <c r="R24" t="str">
+        <f t="shared" ref="R24" si="23">Q24</f>
+        <v>0445</v>
+      </c>
+      <c r="S24" t="str">
+        <f t="shared" ref="S24" si="24">"0x"&amp;R24</f>
+        <v>0x0445</v>
+      </c>
+      <c r="U24" s="3">
         <v>0.47</v>
       </c>
-      <c r="U24" s="4">
+      <c r="V24" s="4">
         <v>0.88</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2191,24 +2300,24 @@
         <v>1</v>
       </c>
       <c r="O25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1349</v>
       </c>
       <c r="Q25" t="str">
         <f t="shared" si="1"/>
         <v>0545</v>
       </c>
-      <c r="T25" s="3">
+      <c r="U25" s="3">
         <v>0.43</v>
       </c>
-      <c r="U25" s="7">
+      <c r="V25" s="7">
         <v>0.9</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2249,24 +2358,32 @@
         <v>1</v>
       </c>
       <c r="O26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1349</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" si="1"/>
         <v>0545</v>
       </c>
-      <c r="T26" s="3">
+      <c r="R26" t="str">
+        <f t="shared" ref="R26" si="25">Q26</f>
+        <v>0545</v>
+      </c>
+      <c r="S26" t="str">
+        <f t="shared" ref="S26" si="26">"0x"&amp;R26</f>
+        <v>0x0545</v>
+      </c>
+      <c r="U26" s="3">
         <v>0.38</v>
       </c>
-      <c r="U26" s="7">
+      <c r="V26" s="7">
         <v>0.92</v>
       </c>
-      <c r="V26">
+      <c r="W26">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2307,24 +2424,24 @@
         <v>1</v>
       </c>
       <c r="O27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1349</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" si="1"/>
         <v>0545</v>
       </c>
-      <c r="T27" s="3">
+      <c r="U27" s="3">
         <v>0.34</v>
       </c>
-      <c r="U27" s="7">
+      <c r="V27" s="7">
         <v>0.94</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2365,24 +2482,32 @@
         <v>1</v>
       </c>
       <c r="O28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1345</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" si="1"/>
         <v>0541</v>
       </c>
-      <c r="T28" s="2">
+      <c r="R28" t="str">
+        <f t="shared" ref="R28" si="27">Q28</f>
+        <v>0541</v>
+      </c>
+      <c r="S28" t="str">
+        <f t="shared" ref="S28" si="28">"0x"&amp;R28</f>
+        <v>0x0541</v>
+      </c>
+      <c r="U28" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U28" s="7">
+      <c r="V28" s="7">
         <v>0.96</v>
       </c>
-      <c r="V28">
+      <c r="W28">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2423,24 +2548,24 @@
         <v>1</v>
       </c>
       <c r="O29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1601</v>
       </c>
       <c r="Q29" t="str">
         <f t="shared" si="1"/>
         <v>0641</v>
       </c>
-      <c r="T29" s="2">
+      <c r="U29" s="2">
         <v>0.24</v>
       </c>
-      <c r="U29" s="8">
+      <c r="V29" s="8">
         <v>0.97</v>
       </c>
-      <c r="V29">
+      <c r="W29">
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2481,24 +2606,32 @@
         <v>1</v>
       </c>
       <c r="O30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1601</v>
       </c>
       <c r="Q30" t="str">
         <f t="shared" si="1"/>
         <v>0641</v>
       </c>
-      <c r="T30" s="2">
+      <c r="R30" t="str">
+        <f t="shared" ref="R30" si="29">Q30</f>
+        <v>0641</v>
+      </c>
+      <c r="S30" t="str">
+        <f t="shared" ref="S30" si="30">"0x"&amp;R30</f>
+        <v>0x0641</v>
+      </c>
+      <c r="U30" s="2">
         <v>0.2</v>
       </c>
-      <c r="U30" s="8">
+      <c r="V30" s="8">
         <v>0.98</v>
       </c>
-      <c r="V30">
+      <c r="W30">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2539,24 +2672,24 @@
         <v>1</v>
       </c>
       <c r="O31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1601</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="1"/>
         <v>0641</v>
       </c>
-      <c r="T31" s="2">
+      <c r="U31" s="2">
         <v>0.15</v>
       </c>
-      <c r="U31" s="8">
+      <c r="V31" s="8">
         <v>0.99</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2597,24 +2730,32 @@
         <v>0</v>
       </c>
       <c r="O32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1600</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="1"/>
         <v>0640</v>
       </c>
-      <c r="T32" s="1">
+      <c r="R32" t="str">
+        <f t="shared" ref="R32" si="31">Q32</f>
+        <v>0640</v>
+      </c>
+      <c r="S32" t="str">
+        <f t="shared" ref="S32" si="32">"0x"&amp;R32</f>
+        <v>0x0640</v>
+      </c>
+      <c r="U32" s="1">
         <v>0.1</v>
       </c>
-      <c r="U32" s="8">
-        <v>1</v>
-      </c>
-      <c r="V32">
+      <c r="V32" s="8">
+        <v>1</v>
+      </c>
+      <c r="W32">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2655,24 +2796,24 @@
         <v>0</v>
       </c>
       <c r="O33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1856</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="1"/>
         <v>0740</v>
       </c>
-      <c r="T33" s="1">
+      <c r="U33" s="1">
         <v>0.05</v>
       </c>
-      <c r="U33" s="10">
-        <v>1</v>
-      </c>
-      <c r="V33">
+      <c r="V33" s="10">
+        <v>1</v>
+      </c>
+      <c r="W33">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2713,24 +2854,32 @@
         <v>0</v>
       </c>
       <c r="O34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1856</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="1"/>
         <v>0740</v>
       </c>
-      <c r="T34" s="1">
-        <v>0</v>
-      </c>
-      <c r="U34" s="10">
-        <v>1</v>
-      </c>
-      <c r="V34">
+      <c r="R34" t="str">
+        <f t="shared" ref="R34" si="33">Q34</f>
+        <v>0740</v>
+      </c>
+      <c r="S34" t="str">
+        <f t="shared" ref="S34" si="34">"0x"&amp;R34</f>
+        <v>0x0740</v>
+      </c>
+      <c r="U34" s="1">
+        <v>0</v>
+      </c>
+      <c r="V34" s="10">
+        <v>1</v>
+      </c>
+      <c r="W34">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2771,24 +2920,24 @@
         <v>0</v>
       </c>
       <c r="O35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1858</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="1"/>
         <v>0742</v>
       </c>
-      <c r="T35" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="U35" s="10">
-        <v>1</v>
-      </c>
-      <c r="V35">
+      <c r="U35" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="V35" s="10">
+        <v>1</v>
+      </c>
+      <c r="W35">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2829,24 +2978,32 @@
         <v>0</v>
       </c>
       <c r="O36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1602</v>
       </c>
       <c r="Q36" t="str">
         <f t="shared" si="1"/>
         <v>0642</v>
       </c>
-      <c r="T36" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="U36" s="8">
-        <v>1</v>
-      </c>
-      <c r="V36">
+      <c r="R36" t="str">
+        <f t="shared" ref="R36" si="35">Q36</f>
+        <v>0642</v>
+      </c>
+      <c r="S36" t="str">
+        <f t="shared" ref="S36" si="36">"0x"&amp;R36</f>
+        <v>0x0642</v>
+      </c>
+      <c r="U36" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="V36" s="8">
+        <v>1</v>
+      </c>
+      <c r="W36">
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2887,24 +3044,24 @@
         <v>1</v>
       </c>
       <c r="O37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1603</v>
       </c>
       <c r="Q37" t="str">
         <f t="shared" si="1"/>
         <v>0643</v>
       </c>
-      <c r="T37" s="18" t="s">
+      <c r="U37" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="U37" s="8">
+      <c r="V37" s="8">
         <v>0.99</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2945,24 +3102,32 @@
         <v>1</v>
       </c>
       <c r="O38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1603</v>
       </c>
       <c r="Q38" t="str">
         <f t="shared" si="1"/>
         <v>0643</v>
       </c>
-      <c r="T38" s="18" t="s">
+      <c r="R38" t="str">
+        <f t="shared" ref="R38" si="37">Q38</f>
+        <v>0643</v>
+      </c>
+      <c r="S38" t="str">
+        <f t="shared" ref="S38" si="38">"0x"&amp;R38</f>
+        <v>0x0643</v>
+      </c>
+      <c r="U38" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="U38" s="8">
+      <c r="V38" s="8">
         <v>0.98</v>
       </c>
-      <c r="V38">
+      <c r="W38">
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3003,24 +3168,24 @@
         <v>1</v>
       </c>
       <c r="O39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1603</v>
       </c>
       <c r="Q39" t="str">
         <f t="shared" si="1"/>
         <v>0643</v>
       </c>
-      <c r="T39" s="18" t="s">
+      <c r="U39" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="U39" s="8">
+      <c r="V39" s="8">
         <v>0.97</v>
       </c>
-      <c r="V39">
+      <c r="W39">
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3061,24 +3226,32 @@
         <v>1</v>
       </c>
       <c r="O40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1347</v>
       </c>
       <c r="Q40" t="str">
         <f t="shared" si="1"/>
         <v>0543</v>
       </c>
-      <c r="T40" s="18" t="s">
+      <c r="R40" t="str">
+        <f t="shared" ref="R40" si="39">Q40</f>
+        <v>0543</v>
+      </c>
+      <c r="S40" t="str">
+        <f t="shared" ref="S40" si="40">"0x"&amp;R40</f>
+        <v>0x0543</v>
+      </c>
+      <c r="U40" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="U40" s="7">
+      <c r="V40" s="7">
         <v>0.96</v>
       </c>
-      <c r="V40">
+      <c r="W40">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3119,24 +3292,24 @@
         <v>1</v>
       </c>
       <c r="O41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1351</v>
       </c>
       <c r="Q41" t="str">
         <f t="shared" si="1"/>
         <v>0547</v>
       </c>
-      <c r="T41" s="17" t="s">
+      <c r="U41" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="U41" s="7">
+      <c r="V41" s="7">
         <v>0.94</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3177,24 +3350,32 @@
         <v>1</v>
       </c>
       <c r="O42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1351</v>
       </c>
       <c r="Q42" t="str">
         <f t="shared" si="1"/>
         <v>0547</v>
       </c>
-      <c r="T42" s="17" t="s">
+      <c r="R42" t="str">
+        <f t="shared" ref="R42" si="41">Q42</f>
+        <v>0547</v>
+      </c>
+      <c r="S42" t="str">
+        <f t="shared" ref="S42" si="42">"0x"&amp;R42</f>
+        <v>0x0547</v>
+      </c>
+      <c r="U42" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="U42" s="7">
+      <c r="V42" s="7">
         <v>0.92</v>
       </c>
-      <c r="V42">
+      <c r="W42">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3235,24 +3416,24 @@
         <v>1</v>
       </c>
       <c r="O43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1351</v>
       </c>
       <c r="Q43" t="str">
         <f t="shared" si="1"/>
         <v>0547</v>
       </c>
-      <c r="T43" s="17" t="s">
+      <c r="U43" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="U43" s="7">
+      <c r="V43" s="7">
         <v>0.9</v>
       </c>
-      <c r="V43">
+      <c r="W43">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3293,24 +3474,32 @@
         <v>1</v>
       </c>
       <c r="O44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1095</v>
       </c>
       <c r="Q44" t="str">
         <f t="shared" si="1"/>
         <v>0447</v>
       </c>
-      <c r="T44" s="17" t="s">
+      <c r="R44" t="str">
+        <f t="shared" ref="R44" si="43">Q44</f>
+        <v>0447</v>
+      </c>
+      <c r="S44" t="str">
+        <f t="shared" ref="S44" si="44">"0x"&amp;R44</f>
+        <v>0x0447</v>
+      </c>
+      <c r="U44" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U44" s="4">
+      <c r="V44" s="4">
         <v>0.88</v>
       </c>
-      <c r="V44">
+      <c r="W44">
         <v>118</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3351,24 +3540,24 @@
         <v>1</v>
       </c>
       <c r="O45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1099</v>
       </c>
       <c r="Q45" t="str">
         <f t="shared" si="1"/>
         <v>044B</v>
       </c>
-      <c r="T45" s="6" t="s">
+      <c r="U45" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="U45" s="4">
+      <c r="V45" s="4">
         <v>0.86</v>
       </c>
-      <c r="V45">
+      <c r="W45">
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3409,24 +3598,32 @@
         <v>1</v>
       </c>
       <c r="O46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1099</v>
       </c>
       <c r="Q46" t="str">
         <f t="shared" si="1"/>
         <v>044B</v>
       </c>
-      <c r="T46" s="6" t="s">
+      <c r="R46" t="str">
+        <f t="shared" ref="R46" si="45">Q46</f>
+        <v>044B</v>
+      </c>
+      <c r="S46" t="str">
+        <f t="shared" ref="S46" si="46">"0x"&amp;R46</f>
+        <v>0x044B</v>
+      </c>
+      <c r="U46" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="U46" s="4">
+      <c r="V46" s="4">
         <v>0.83</v>
       </c>
-      <c r="V46">
+      <c r="W46">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3467,24 +3664,24 @@
         <v>1</v>
       </c>
       <c r="O47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>1099</v>
       </c>
       <c r="Q47" t="str">
         <f t="shared" si="1"/>
         <v>044B</v>
       </c>
-      <c r="T47" s="6" t="s">
+      <c r="U47" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="U47" s="4">
+      <c r="V47" s="4">
         <v>0.8</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3525,24 +3722,32 @@
         <v>1</v>
       </c>
       <c r="O48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>843</v>
       </c>
       <c r="Q48" t="str">
         <f t="shared" si="1"/>
         <v>034B</v>
       </c>
-      <c r="T48" s="6" t="s">
+      <c r="R48" t="str">
+        <f t="shared" ref="R48" si="47">Q48</f>
+        <v>034B</v>
+      </c>
+      <c r="S48" t="str">
+        <f t="shared" ref="S48" si="48">"0x"&amp;R48</f>
+        <v>0x034B</v>
+      </c>
+      <c r="U48" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="U48" s="5">
+      <c r="V48" s="5">
         <v>0.77</v>
       </c>
-      <c r="V48">
+      <c r="W48">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3583,24 +3788,24 @@
         <v>1</v>
       </c>
       <c r="O49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>847</v>
       </c>
       <c r="Q49" t="str">
         <f t="shared" si="1"/>
         <v>034F</v>
       </c>
-      <c r="T49" s="5" t="s">
+      <c r="U49" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="U49" s="5">
+      <c r="V49" s="5">
         <v>0.74</v>
       </c>
-      <c r="V49">
+      <c r="W49">
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3641,24 +3846,32 @@
         <v>1</v>
       </c>
       <c r="O50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>847</v>
       </c>
       <c r="Q50" t="str">
         <f t="shared" si="1"/>
         <v>034F</v>
       </c>
-      <c r="T50" s="5" t="s">
+      <c r="R50" t="str">
+        <f t="shared" ref="R50" si="49">Q50</f>
+        <v>034F</v>
+      </c>
+      <c r="S50" t="str">
+        <f t="shared" ref="S50" si="50">"0x"&amp;R50</f>
+        <v>0x034F</v>
+      </c>
+      <c r="U50" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U50" s="5">
+      <c r="V50" s="5">
         <v>0.71</v>
       </c>
-      <c r="V50">
+      <c r="W50">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3699,24 +3912,24 @@
         <v>1</v>
       </c>
       <c r="O51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>847</v>
       </c>
       <c r="Q51" t="str">
         <f t="shared" si="1"/>
         <v>034F</v>
       </c>
-      <c r="T51" s="5" t="s">
+      <c r="U51" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="U51" s="5">
+      <c r="V51" s="5">
         <v>0.67</v>
       </c>
-      <c r="V51">
+      <c r="W51">
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3757,24 +3970,32 @@
         <v>1</v>
       </c>
       <c r="O52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>591</v>
       </c>
       <c r="Q52" t="str">
         <f t="shared" si="1"/>
         <v>024F</v>
       </c>
-      <c r="T52" s="5" t="s">
+      <c r="R52" t="str">
+        <f t="shared" ref="R52" si="51">Q52</f>
+        <v>024F</v>
+      </c>
+      <c r="S52" t="str">
+        <f t="shared" ref="S52" si="52">"0x"&amp;R52</f>
+        <v>0x024F</v>
+      </c>
+      <c r="U52" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="U52" s="6">
+      <c r="V52" s="6">
         <v>0.63</v>
       </c>
-      <c r="V52">
+      <c r="W52">
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3815,24 +4036,24 @@
         <v>1</v>
       </c>
       <c r="O53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>595</v>
       </c>
       <c r="Q53" t="str">
         <f t="shared" si="1"/>
         <v>0253</v>
       </c>
-      <c r="T53" s="4" t="s">
+      <c r="U53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U53" s="6">
+      <c r="V53" s="6">
         <v>0.6</v>
       </c>
-      <c r="V53">
+      <c r="W53">
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3873,24 +4094,32 @@
         <v>1</v>
       </c>
       <c r="O54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>595</v>
       </c>
       <c r="Q54" t="str">
         <f t="shared" si="1"/>
         <v>0253</v>
       </c>
-      <c r="T54" s="4" t="s">
+      <c r="R54" t="str">
+        <f t="shared" ref="R54" si="53">Q54</f>
+        <v>0253</v>
+      </c>
+      <c r="S54" t="str">
+        <f t="shared" ref="S54" si="54">"0x"&amp;R54</f>
+        <v>0x0253</v>
+      </c>
+      <c r="U54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="U54" s="6">
+      <c r="V54" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="V54">
+      <c r="W54">
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3931,24 +4160,24 @@
         <v>1</v>
       </c>
       <c r="O55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>595</v>
       </c>
       <c r="Q55" t="str">
         <f t="shared" si="1"/>
         <v>0253</v>
       </c>
-      <c r="T55" s="4" t="s">
+      <c r="U55" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U55" s="6">
+      <c r="V55" s="6">
         <v>0.51</v>
       </c>
-      <c r="V55">
+      <c r="W55">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3989,24 +4218,32 @@
         <v>1</v>
       </c>
       <c r="O56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>339</v>
       </c>
       <c r="Q56" t="str">
         <f t="shared" si="1"/>
         <v>0153</v>
       </c>
-      <c r="T56" s="4" t="s">
+      <c r="R56" t="str">
+        <f t="shared" ref="R56" si="55">Q56</f>
+        <v>0153</v>
+      </c>
+      <c r="S56" t="str">
+        <f t="shared" ref="S56" si="56">"0x"&amp;R56</f>
+        <v>0x0153</v>
+      </c>
+      <c r="U56" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="U56" s="3">
+      <c r="V56" s="3">
         <v>0.47</v>
       </c>
-      <c r="V56">
+      <c r="W56">
         <v>152</v>
       </c>
     </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4047,24 +4284,24 @@
         <v>1</v>
       </c>
       <c r="O57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>343</v>
       </c>
       <c r="Q57" t="str">
         <f t="shared" si="1"/>
         <v>0157</v>
       </c>
-      <c r="T57" s="7" t="s">
+      <c r="U57" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="U57" s="3">
+      <c r="V57" s="3">
         <v>0.43</v>
       </c>
-      <c r="V57">
+      <c r="W57">
         <v>155</v>
       </c>
     </row>
-    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4105,24 +4342,32 @@
         <v>1</v>
       </c>
       <c r="O58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>343</v>
       </c>
       <c r="Q58" t="str">
         <f t="shared" si="1"/>
         <v>0157</v>
       </c>
-      <c r="T58" s="7" t="s">
+      <c r="R58" t="str">
+        <f t="shared" ref="R58" si="57">Q58</f>
+        <v>0157</v>
+      </c>
+      <c r="S58" t="str">
+        <f t="shared" ref="S58" si="58">"0x"&amp;R58</f>
+        <v>0x0157</v>
+      </c>
+      <c r="U58" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="U58" s="3">
+      <c r="V58" s="3">
         <v>0.38</v>
       </c>
-      <c r="V58">
+      <c r="W58">
         <v>158</v>
       </c>
     </row>
-    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4163,24 +4408,24 @@
         <v>1</v>
       </c>
       <c r="O59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>343</v>
       </c>
       <c r="Q59" t="str">
         <f t="shared" si="1"/>
         <v>0157</v>
       </c>
-      <c r="T59" s="7" t="s">
+      <c r="U59" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="U59" s="3">
+      <c r="V59" s="3">
         <v>0.34</v>
       </c>
-      <c r="V59">
+      <c r="W59">
         <v>160</v>
       </c>
     </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4221,24 +4466,32 @@
         <v>1</v>
       </c>
       <c r="O60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>87</v>
       </c>
       <c r="Q60" t="str">
         <f t="shared" si="1"/>
         <v>0057</v>
       </c>
-      <c r="T60" s="7" t="s">
+      <c r="R60" t="str">
+        <f t="shared" ref="R60" si="59">Q60</f>
+        <v>0057</v>
+      </c>
+      <c r="S60" t="str">
+        <f t="shared" ref="S60" si="60">"0x"&amp;R60</f>
+        <v>0x0057</v>
+      </c>
+      <c r="U60" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="U60" s="2">
+      <c r="V60" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="V60">
+      <c r="W60">
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4279,24 +4532,24 @@
         <v>1</v>
       </c>
       <c r="O61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="Q61" t="str">
         <f t="shared" si="1"/>
         <v>005B</v>
       </c>
-      <c r="T61" s="8" t="s">
+      <c r="U61" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="U61" s="2">
+      <c r="V61" s="2">
         <v>0.24</v>
       </c>
-      <c r="V61">
+      <c r="W61">
         <v>166</v>
       </c>
     </row>
-    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4337,24 +4590,32 @@
         <v>1</v>
       </c>
       <c r="O62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="Q62" t="str">
         <f t="shared" si="1"/>
         <v>005B</v>
       </c>
-      <c r="T62" s="8" t="s">
+      <c r="R62" t="str">
+        <f t="shared" ref="R62" si="61">Q62</f>
+        <v>005B</v>
+      </c>
+      <c r="S62" t="str">
+        <f t="shared" ref="S62" si="62">"0x"&amp;R62</f>
+        <v>0x005B</v>
+      </c>
+      <c r="U62" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="U62" s="2">
+      <c r="V62" s="2">
         <v>0.2</v>
       </c>
-      <c r="V62">
+      <c r="W62">
         <v>169</v>
       </c>
     </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4395,24 +4656,24 @@
         <v>1</v>
       </c>
       <c r="O63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>91</v>
       </c>
       <c r="Q63" t="str">
         <f t="shared" si="1"/>
         <v>005B</v>
       </c>
-      <c r="T63" s="8" t="s">
+      <c r="U63" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="U63" s="2">
+      <c r="V63" s="2">
         <v>0.15</v>
       </c>
-      <c r="V63">
+      <c r="W63">
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4453,24 +4714,32 @@
         <v>1</v>
       </c>
       <c r="O64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>27</v>
       </c>
       <c r="Q64" t="str">
         <f t="shared" si="1"/>
         <v>001B</v>
       </c>
-      <c r="T64" s="8" t="s">
+      <c r="R64" t="str">
+        <f t="shared" ref="R64" si="63">Q64</f>
+        <v>001B</v>
+      </c>
+      <c r="S64" t="str">
+        <f t="shared" ref="S64" si="64">"0x"&amp;R64</f>
+        <v>0x001B</v>
+      </c>
+      <c r="U64" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="U64" s="1">
+      <c r="V64" s="1">
         <v>0.1</v>
       </c>
-      <c r="V64">
+      <c r="W64">
         <v>174</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4511,24 +4780,24 @@
         <v>1</v>
       </c>
       <c r="O65">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="Q65" t="str">
         <f t="shared" si="1"/>
         <v>001F</v>
       </c>
-      <c r="T65" s="10" t="s">
+      <c r="U65" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U65" s="1">
+      <c r="V65" s="1">
         <v>0.05</v>
       </c>
-      <c r="V65">
+      <c r="W65">
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4569,24 +4838,32 @@
         <v>1</v>
       </c>
       <c r="O66">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>31</v>
       </c>
       <c r="Q66" t="str">
         <f t="shared" si="1"/>
         <v>001F</v>
       </c>
-      <c r="T66" s="10" t="s">
+      <c r="R66" t="str">
+        <f t="shared" ref="R66" si="65">Q66</f>
+        <v>001F</v>
+      </c>
+      <c r="S66" t="str">
+        <f t="shared" ref="S66" si="66">"0x"&amp;R66</f>
+        <v>0x001F</v>
+      </c>
+      <c r="U66" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U66" s="1">
-        <v>0</v>
-      </c>
-      <c r="V66">
+      <c r="V66" s="1">
+        <v>0</v>
+      </c>
+      <c r="W66">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4627,24 +4904,24 @@
         <v>1</v>
       </c>
       <c r="O67">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>159</v>
       </c>
       <c r="Q67" t="str">
-        <f t="shared" ref="Q67:Q129" si="3">DEC2HEX(O67,4)</f>
+        <f t="shared" ref="Q67:Q129" si="67">DEC2HEX(O67,4)</f>
         <v>009F</v>
       </c>
-      <c r="T67" s="10" t="s">
+      <c r="U67" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="U67" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="V67">
+      <c r="V67" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="W67">
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4685,24 +4962,32 @@
         <v>1</v>
       </c>
       <c r="O68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>155</v>
       </c>
       <c r="Q68" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>009B</v>
       </c>
-      <c r="T68" s="11" t="s">
+      <c r="R68" t="str">
+        <f t="shared" ref="R68" si="68">Q68</f>
+        <v>009B</v>
+      </c>
+      <c r="S68" t="str">
+        <f t="shared" ref="S68" si="69">"0x"&amp;R68</f>
+        <v>0x009B</v>
+      </c>
+      <c r="U68" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="U68" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="V68">
+      <c r="V68" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W68">
         <v>186</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4743,24 +5028,24 @@
         <v>1</v>
       </c>
       <c r="O69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>155</v>
       </c>
       <c r="Q69" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>009B</v>
       </c>
-      <c r="T69" s="11" t="s">
+      <c r="U69" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="U69" s="19" t="s">
+      <c r="V69" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="V69">
+      <c r="W69">
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4801,24 +5086,32 @@
         <v>1</v>
       </c>
       <c r="O70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>219</v>
       </c>
       <c r="Q70" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00DB</v>
       </c>
-      <c r="T70" s="11" t="s">
+      <c r="R70" t="str">
+        <f t="shared" ref="R70" si="70">Q70</f>
+        <v>00DB</v>
+      </c>
+      <c r="S70" t="str">
+        <f t="shared" ref="S70" si="71">"0x"&amp;R70</f>
+        <v>0x00DB</v>
+      </c>
+      <c r="U70" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="U70" s="18" t="s">
+      <c r="V70" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="V70">
+      <c r="W70">
         <v>191</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4859,24 +5152,24 @@
         <v>1</v>
       </c>
       <c r="O71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>219</v>
       </c>
       <c r="Q71" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00DB</v>
       </c>
-      <c r="T71" s="11" t="s">
+      <c r="U71" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="U71" s="18" t="s">
+      <c r="V71" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="V71">
+      <c r="W71">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4917,24 +5210,32 @@
         <v>1</v>
       </c>
       <c r="O72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>215</v>
       </c>
       <c r="Q72" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00D7</v>
       </c>
-      <c r="T72" s="13" t="s">
+      <c r="R72" t="str">
+        <f t="shared" ref="R72" si="72">Q72</f>
+        <v>00D7</v>
+      </c>
+      <c r="S72" t="str">
+        <f t="shared" ref="S72" si="73">"0x"&amp;R72</f>
+        <v>0x00D7</v>
+      </c>
+      <c r="U72" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="U72" s="18" t="s">
+      <c r="V72" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="V72">
+      <c r="W72">
         <v>197</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4975,24 +5276,24 @@
         <v>1</v>
       </c>
       <c r="O73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>471</v>
       </c>
       <c r="Q73" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D7</v>
       </c>
-      <c r="T73" s="13" t="s">
+      <c r="U73" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="U73" s="17" t="s">
+      <c r="V73" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="V73">
+      <c r="W73">
         <v>200</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -5033,24 +5334,32 @@
         <v>1</v>
       </c>
       <c r="O74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>471</v>
       </c>
       <c r="Q74" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D7</v>
       </c>
-      <c r="T74" s="13" t="s">
+      <c r="R74" t="str">
+        <f t="shared" ref="R74" si="74">Q74</f>
+        <v>01D7</v>
+      </c>
+      <c r="S74" t="str">
+        <f t="shared" ref="S74" si="75">"0x"&amp;R74</f>
+        <v>0x01D7</v>
+      </c>
+      <c r="U74" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="U74" s="17" t="s">
+      <c r="V74" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="V74">
+      <c r="W74">
         <v>203</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -5091,24 +5400,24 @@
         <v>1</v>
       </c>
       <c r="O75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>471</v>
       </c>
       <c r="Q75" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D7</v>
       </c>
-      <c r="T75" s="13" t="s">
+      <c r="U75" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="U75" s="17" t="s">
+      <c r="V75" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="V75">
+      <c r="W75">
         <v>205</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -5149,24 +5458,32 @@
         <v>1</v>
       </c>
       <c r="O76">
-        <f t="shared" ref="O76:O129" si="4">C76*POWER(2,11)+D76*POWER(2,10)+E76*POWER(2,9)+F76*POWER(2,8)+G76*POWER(2,7)+H76*POWER(2,6)+I76*POWER(2,5)+J76*POWER(2,4)+K76*POWER(2,3)+L76*POWER(2,2)+M76*POWER(2,1)+N76*POWER(2,0)</f>
+        <f t="shared" ref="O76:O129" si="76">C76*POWER(2,11)+D76*POWER(2,10)+E76*POWER(2,9)+F76*POWER(2,8)+G76*POWER(2,7)+H76*POWER(2,6)+I76*POWER(2,5)+J76*POWER(2,4)+K76*POWER(2,3)+L76*POWER(2,2)+M76*POWER(2,1)+N76*POWER(2,0)</f>
         <v>467</v>
       </c>
       <c r="Q76" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D3</v>
       </c>
-      <c r="T76" s="14" t="s">
+      <c r="R76" t="str">
+        <f t="shared" ref="R76" si="77">Q76</f>
+        <v>01D3</v>
+      </c>
+      <c r="S76" t="str">
+        <f t="shared" ref="S76" si="78">"0x"&amp;R76</f>
+        <v>0x01D3</v>
+      </c>
+      <c r="U76" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="U76" s="17" t="s">
+      <c r="V76" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="V76">
+      <c r="W76">
         <v>208</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -5207,24 +5524,24 @@
         <v>1</v>
       </c>
       <c r="O77">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>723</v>
       </c>
       <c r="Q77" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D3</v>
       </c>
-      <c r="T77" s="14" t="s">
+      <c r="U77" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="U77" s="16" t="s">
+      <c r="V77" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="V77">
+      <c r="W77">
         <v>211</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -5265,24 +5582,32 @@
         <v>1</v>
       </c>
       <c r="O78">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>723</v>
       </c>
       <c r="Q78" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D3</v>
       </c>
-      <c r="T78" s="14" t="s">
+      <c r="R78" t="str">
+        <f t="shared" ref="R78" si="79">Q78</f>
+        <v>02D3</v>
+      </c>
+      <c r="S78" t="str">
+        <f t="shared" ref="S78" si="80">"0x"&amp;R78</f>
+        <v>0x02D3</v>
+      </c>
+      <c r="U78" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="U78" s="16" t="s">
+      <c r="V78" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="V78">
+      <c r="W78">
         <v>214</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -5323,24 +5648,24 @@
         <v>1</v>
       </c>
       <c r="O79">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>723</v>
       </c>
       <c r="Q79" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D3</v>
       </c>
-      <c r="T79" s="14" t="s">
+      <c r="U79" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="U79" s="16" t="s">
+      <c r="V79" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="V79">
+      <c r="W79">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -5381,24 +5706,32 @@
         <v>1</v>
       </c>
       <c r="O80">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>719</v>
       </c>
       <c r="Q80" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02CF</v>
       </c>
-      <c r="T80" s="15" t="s">
+      <c r="R80" t="str">
+        <f t="shared" ref="R80" si="81">Q80</f>
+        <v>02CF</v>
+      </c>
+      <c r="S80" t="str">
+        <f t="shared" ref="S80" si="82">"0x"&amp;R80</f>
+        <v>0x02CF</v>
+      </c>
+      <c r="U80" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="U80" s="16" t="s">
+      <c r="V80" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="V80">
+      <c r="W80">
         <v>219</v>
       </c>
     </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -5439,24 +5772,24 @@
         <v>1</v>
       </c>
       <c r="O81">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>975</v>
       </c>
       <c r="Q81" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CF</v>
       </c>
-      <c r="T81" s="15" t="s">
+      <c r="U81" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="U81" s="15" t="s">
+      <c r="V81" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="V81">
+      <c r="W81">
         <v>222</v>
       </c>
     </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5497,24 +5830,32 @@
         <v>1</v>
       </c>
       <c r="O82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>975</v>
       </c>
       <c r="Q82" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CF</v>
       </c>
-      <c r="T82" s="15" t="s">
-        <v>16</v>
+      <c r="R82" t="str">
+        <f t="shared" ref="R82" si="83">Q82</f>
+        <v>03CF</v>
+      </c>
+      <c r="S82" t="str">
+        <f t="shared" ref="S82" si="84">"0x"&amp;R82</f>
+        <v>0x03CF</v>
       </c>
       <c r="U82" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="V82">
+      <c r="V82" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="W82">
         <v>225</v>
       </c>
     </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5555,24 +5896,24 @@
         <v>1</v>
       </c>
       <c r="O83">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>975</v>
       </c>
       <c r="Q83" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CF</v>
       </c>
-      <c r="T83" s="15" t="s">
+      <c r="U83" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="U83" s="15" t="s">
+      <c r="V83" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="V83">
+      <c r="W83">
         <v>228</v>
       </c>
     </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5613,24 +5954,32 @@
         <v>1</v>
       </c>
       <c r="O84">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>971</v>
       </c>
       <c r="Q84" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CB</v>
       </c>
-      <c r="T84" s="16" t="s">
+      <c r="R84" t="str">
+        <f t="shared" ref="R84" si="85">Q84</f>
+        <v>03CB</v>
+      </c>
+      <c r="S84" t="str">
+        <f t="shared" ref="S84" si="86">"0x"&amp;R84</f>
+        <v>0x03CB</v>
+      </c>
+      <c r="U84" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="U84" s="15" t="s">
+      <c r="V84" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="V84">
+      <c r="W84">
         <v>231</v>
       </c>
     </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5671,24 +6020,24 @@
         <v>1</v>
       </c>
       <c r="O85">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1227</v>
       </c>
       <c r="Q85" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04CB</v>
       </c>
-      <c r="T85" s="16" t="s">
+      <c r="U85" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="U85" s="14" t="s">
+      <c r="V85" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="V85">
+      <c r="W85">
         <v>233</v>
       </c>
     </row>
-    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5729,24 +6078,32 @@
         <v>1</v>
       </c>
       <c r="O86">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1227</v>
       </c>
       <c r="Q86" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04CB</v>
       </c>
-      <c r="T86" s="16" t="s">
+      <c r="R86" t="str">
+        <f t="shared" ref="R86" si="87">Q86</f>
+        <v>04CB</v>
+      </c>
+      <c r="S86" t="str">
+        <f t="shared" ref="S86" si="88">"0x"&amp;R86</f>
+        <v>0x04CB</v>
+      </c>
+      <c r="U86" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="U86" s="14" t="s">
+      <c r="V86" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="V86">
+      <c r="W86">
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5787,24 +6144,24 @@
         <v>1</v>
       </c>
       <c r="O87">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1227</v>
       </c>
       <c r="Q87" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04CB</v>
       </c>
-      <c r="T87" s="16" t="s">
+      <c r="U87" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="U87" s="14" t="s">
+      <c r="V87" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V87">
+      <c r="W87">
         <v>239</v>
       </c>
     </row>
-    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5845,24 +6202,32 @@
         <v>1</v>
       </c>
       <c r="O88">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1223</v>
       </c>
       <c r="Q88" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04C7</v>
       </c>
-      <c r="T88" s="17" t="s">
+      <c r="R88" t="str">
+        <f t="shared" ref="R88" si="89">Q88</f>
+        <v>04C7</v>
+      </c>
+      <c r="S88" t="str">
+        <f t="shared" ref="S88" si="90">"0x"&amp;R88</f>
+        <v>0x04C7</v>
+      </c>
+      <c r="U88" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="U88" s="14" t="s">
+      <c r="V88" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="V88">
+      <c r="W88">
         <v>242</v>
       </c>
     </row>
-    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5903,24 +6268,24 @@
         <v>1</v>
       </c>
       <c r="O89">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1479</v>
       </c>
       <c r="Q89" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C7</v>
       </c>
-      <c r="T89" s="17" t="s">
+      <c r="U89" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="U89" s="13" t="s">
+      <c r="V89" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V89">
+      <c r="W89">
         <v>245</v>
       </c>
     </row>
-    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5961,24 +6326,32 @@
         <v>1</v>
       </c>
       <c r="O90">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1479</v>
       </c>
       <c r="Q90" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C7</v>
       </c>
-      <c r="T90" s="17" t="s">
+      <c r="R90" t="str">
+        <f t="shared" ref="R90" si="91">Q90</f>
+        <v>05C7</v>
+      </c>
+      <c r="S90" t="str">
+        <f t="shared" ref="S90" si="92">"0x"&amp;R90</f>
+        <v>0x05C7</v>
+      </c>
+      <c r="U90" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="U90" s="13" t="s">
+      <c r="V90" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V90">
+      <c r="W90">
         <v>248</v>
       </c>
     </row>
-    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6019,24 +6392,24 @@
         <v>1</v>
       </c>
       <c r="O91">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1479</v>
       </c>
       <c r="Q91" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C7</v>
       </c>
-      <c r="T91" s="17" t="s">
+      <c r="U91" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="U91" s="13" t="s">
+      <c r="V91" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="V91">
+      <c r="W91">
         <v>250</v>
       </c>
     </row>
-    <row r="92" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6077,24 +6450,32 @@
         <v>1</v>
       </c>
       <c r="O92">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1475</v>
       </c>
       <c r="Q92" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C3</v>
       </c>
-      <c r="T92" s="18" t="s">
+      <c r="R92" t="str">
+        <f t="shared" ref="R92" si="93">Q92</f>
+        <v>05C3</v>
+      </c>
+      <c r="S92" t="str">
+        <f t="shared" ref="S92" si="94">"0x"&amp;R92</f>
+        <v>0x05C3</v>
+      </c>
+      <c r="U92" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="U92" s="13" t="s">
+      <c r="V92" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="V92">
+      <c r="W92">
         <v>253</v>
       </c>
     </row>
-    <row r="93" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6135,24 +6516,24 @@
         <v>1</v>
       </c>
       <c r="O93">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1731</v>
       </c>
       <c r="Q93" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C3</v>
       </c>
-      <c r="T93" s="18" t="s">
+      <c r="U93" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="U93" s="11" t="s">
+      <c r="V93" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V93">
+      <c r="W93">
         <v>256</v>
       </c>
     </row>
-    <row r="94" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6193,24 +6574,32 @@
         <v>1</v>
       </c>
       <c r="O94">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1731</v>
       </c>
       <c r="Q94" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C3</v>
       </c>
-      <c r="T94" s="18" t="s">
+      <c r="R94" t="str">
+        <f t="shared" ref="R94" si="95">Q94</f>
+        <v>06C3</v>
+      </c>
+      <c r="S94" t="str">
+        <f t="shared" ref="S94" si="96">"0x"&amp;R94</f>
+        <v>0x06C3</v>
+      </c>
+      <c r="U94" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="U94" s="11" t="s">
+      <c r="V94" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="V94">
+      <c r="W94">
         <v>259</v>
       </c>
     </row>
-    <row r="95" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6251,24 +6640,24 @@
         <v>1</v>
       </c>
       <c r="O95">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1731</v>
       </c>
       <c r="Q95" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C3</v>
       </c>
-      <c r="T95" s="18" t="s">
+      <c r="U95" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="U95" s="11" t="s">
+      <c r="V95" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="V95">
+      <c r="W95">
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6309,24 +6698,32 @@
         <v>0</v>
       </c>
       <c r="O96">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1730</v>
       </c>
       <c r="Q96" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C2</v>
       </c>
-      <c r="T96" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="U96" s="11" t="s">
+      <c r="R96" t="str">
+        <f t="shared" ref="R96" si="97">Q96</f>
+        <v>06C2</v>
+      </c>
+      <c r="S96" t="str">
+        <f t="shared" ref="S96" si="98">"0x"&amp;R96</f>
+        <v>0x06C2</v>
+      </c>
+      <c r="U96" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="V96" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="V96">
+      <c r="W96">
         <v>264</v>
       </c>
     </row>
-    <row r="97" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6367,24 +6764,24 @@
         <v>0</v>
       </c>
       <c r="O97">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1986</v>
       </c>
       <c r="Q97" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>07C2</v>
       </c>
-      <c r="T97" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="U97" s="12" t="s">
+      <c r="U97" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="V97" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="V97">
+      <c r="W97">
         <v>267</v>
       </c>
     </row>
-    <row r="98" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6425,24 +6822,32 @@
         <v>0</v>
       </c>
       <c r="O98">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1984</v>
       </c>
       <c r="Q98" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>07C0</v>
       </c>
-      <c r="T98" s="20">
-        <v>0</v>
-      </c>
-      <c r="U98" s="12" t="s">
+      <c r="R98" t="str">
+        <f t="shared" ref="R98" si="99">Q98</f>
+        <v>07C0</v>
+      </c>
+      <c r="S98" t="str">
+        <f t="shared" ref="S98" si="100">"0x"&amp;R98</f>
+        <v>0x07C0</v>
+      </c>
+      <c r="U98" s="20">
+        <v>0</v>
+      </c>
+      <c r="V98" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="V98">
+      <c r="W98">
         <v>270</v>
       </c>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6483,24 +6888,24 @@
         <v>0</v>
       </c>
       <c r="O99">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1984</v>
       </c>
       <c r="Q99" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>07C0</v>
       </c>
-      <c r="T99" s="19">
+      <c r="U99" s="19">
         <v>0.05</v>
       </c>
-      <c r="U99" s="12" t="s">
+      <c r="V99" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="V99">
+      <c r="W99">
         <v>273</v>
       </c>
     </row>
-    <row r="100" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6541,24 +6946,32 @@
         <v>0</v>
       </c>
       <c r="O100">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1728</v>
       </c>
       <c r="Q100" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C0</v>
       </c>
-      <c r="T100" s="19">
+      <c r="R100" t="str">
+        <f t="shared" ref="R100" si="101">Q100</f>
+        <v>06C0</v>
+      </c>
+      <c r="S100" t="str">
+        <f t="shared" ref="S100" si="102">"0x"&amp;R100</f>
+        <v>0x06C0</v>
+      </c>
+      <c r="U100" s="19">
         <v>0.1</v>
       </c>
-      <c r="U100" s="11" t="s">
+      <c r="V100" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="V100">
+      <c r="W100">
         <v>276</v>
       </c>
     </row>
-    <row r="101" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6599,24 +7012,24 @@
         <v>1</v>
       </c>
       <c r="O101">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1729</v>
       </c>
       <c r="Q101" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C1</v>
       </c>
-      <c r="T101" s="18">
+      <c r="U101" s="18">
         <v>0.15</v>
       </c>
-      <c r="U101" s="11" t="s">
+      <c r="V101" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="V101">
+      <c r="W101">
         <v>278</v>
       </c>
     </row>
-    <row r="102" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6657,24 +7070,32 @@
         <v>1</v>
       </c>
       <c r="O102">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1729</v>
       </c>
       <c r="Q102" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C1</v>
       </c>
-      <c r="T102" s="18">
+      <c r="R102" t="str">
+        <f t="shared" ref="R102" si="103">Q102</f>
+        <v>06C1</v>
+      </c>
+      <c r="S102" t="str">
+        <f t="shared" ref="S102" si="104">"0x"&amp;R102</f>
+        <v>0x06C1</v>
+      </c>
+      <c r="U102" s="18">
         <v>0.2</v>
       </c>
-      <c r="U102" s="11" t="s">
+      <c r="V102" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="V102">
+      <c r="W102">
         <v>281</v>
       </c>
     </row>
-    <row r="103" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6715,24 +7136,24 @@
         <v>1</v>
       </c>
       <c r="O103">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1729</v>
       </c>
       <c r="Q103" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>06C1</v>
       </c>
-      <c r="T103" s="18">
+      <c r="U103" s="18">
         <v>0.24</v>
       </c>
-      <c r="U103" s="11" t="s">
+      <c r="V103" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="V103">
+      <c r="W103">
         <v>284</v>
       </c>
     </row>
-    <row r="104" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6773,24 +7194,32 @@
         <v>1</v>
       </c>
       <c r="O104">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1473</v>
       </c>
       <c r="Q104" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C1</v>
       </c>
-      <c r="T104" s="18">
+      <c r="R104" t="str">
+        <f t="shared" ref="R104" si="105">Q104</f>
+        <v>05C1</v>
+      </c>
+      <c r="S104" t="str">
+        <f t="shared" ref="S104" si="106">"0x"&amp;R104</f>
+        <v>0x05C1</v>
+      </c>
+      <c r="U104" s="18">
         <v>0.28999999999999998</v>
       </c>
-      <c r="U104" s="13" t="s">
+      <c r="V104" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="V104">
+      <c r="W104">
         <v>287</v>
       </c>
     </row>
-    <row r="105" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6831,24 +7260,24 @@
         <v>1</v>
       </c>
       <c r="O105">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1477</v>
       </c>
       <c r="Q105" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C5</v>
       </c>
-      <c r="T105" s="17">
+      <c r="U105" s="17">
         <v>0.34</v>
       </c>
-      <c r="U105" s="13" t="s">
+      <c r="V105" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="V105">
+      <c r="W105">
         <v>290</v>
       </c>
     </row>
-    <row r="106" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6889,24 +7318,32 @@
         <v>1</v>
       </c>
       <c r="O106">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1477</v>
       </c>
       <c r="Q106" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C5</v>
       </c>
-      <c r="T106" s="17">
+      <c r="R106" t="str">
+        <f t="shared" ref="R106" si="107">Q106</f>
+        <v>05C5</v>
+      </c>
+      <c r="S106" t="str">
+        <f t="shared" ref="S106" si="108">"0x"&amp;R106</f>
+        <v>0x05C5</v>
+      </c>
+      <c r="U106" s="17">
         <v>0.38</v>
       </c>
-      <c r="U106" s="13" t="s">
+      <c r="V106" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="V106">
+      <c r="W106">
         <v>293</v>
       </c>
     </row>
-    <row r="107" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -6947,24 +7384,24 @@
         <v>1</v>
       </c>
       <c r="O107">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1477</v>
       </c>
       <c r="Q107" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>05C5</v>
       </c>
-      <c r="T107" s="17">
+      <c r="U107" s="17">
         <v>0.43</v>
       </c>
-      <c r="U107" s="13" t="s">
+      <c r="V107" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="V107">
+      <c r="W107">
         <v>295</v>
       </c>
     </row>
-    <row r="108" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7005,24 +7442,32 @@
         <v>1</v>
       </c>
       <c r="O108">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1221</v>
       </c>
       <c r="Q108" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04C5</v>
       </c>
-      <c r="T108" s="17">
+      <c r="R108" t="str">
+        <f t="shared" ref="R108" si="109">Q108</f>
+        <v>04C5</v>
+      </c>
+      <c r="S108" t="str">
+        <f t="shared" ref="S108" si="110">"0x"&amp;R108</f>
+        <v>0x04C5</v>
+      </c>
+      <c r="U108" s="17">
         <v>0.47</v>
       </c>
-      <c r="U108" s="14" t="s">
+      <c r="V108" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="V108">
+      <c r="W108">
         <v>298</v>
       </c>
     </row>
-    <row r="109" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7063,24 +7508,24 @@
         <v>1</v>
       </c>
       <c r="O109">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1225</v>
       </c>
       <c r="Q109" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04C9</v>
       </c>
-      <c r="T109" s="6">
+      <c r="U109" s="6">
         <v>0.51</v>
       </c>
-      <c r="U109" s="14" t="s">
+      <c r="V109" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V109">
+      <c r="W109">
         <v>301</v>
       </c>
     </row>
-    <row r="110" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7121,24 +7566,32 @@
         <v>1</v>
       </c>
       <c r="O110">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1225</v>
       </c>
       <c r="Q110" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04C9</v>
       </c>
-      <c r="T110" s="6">
+      <c r="R110" t="str">
+        <f t="shared" ref="R110" si="111">Q110</f>
+        <v>04C9</v>
+      </c>
+      <c r="S110" t="str">
+        <f t="shared" ref="S110" si="112">"0x"&amp;R110</f>
+        <v>0x04C9</v>
+      </c>
+      <c r="U110" s="6">
         <v>0.56000000000000005</v>
       </c>
-      <c r="U110" s="14" t="s">
+      <c r="V110" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="V110">
+      <c r="W110">
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7179,24 +7632,24 @@
         <v>1</v>
       </c>
       <c r="O111">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>1225</v>
       </c>
       <c r="Q111" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>04C9</v>
       </c>
-      <c r="T111" s="6">
+      <c r="U111" s="6">
         <v>0.6</v>
       </c>
-      <c r="U111" s="14" t="s">
+      <c r="V111" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="V111">
+      <c r="W111">
         <v>307</v>
       </c>
     </row>
-    <row r="112" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7237,24 +7690,32 @@
         <v>1</v>
       </c>
       <c r="O112">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>969</v>
       </c>
       <c r="Q112" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03C9</v>
       </c>
-      <c r="T112" s="6">
+      <c r="R112" t="str">
+        <f t="shared" ref="R112" si="113">Q112</f>
+        <v>03C9</v>
+      </c>
+      <c r="S112" t="str">
+        <f t="shared" ref="S112" si="114">"0x"&amp;R112</f>
+        <v>0x03C9</v>
+      </c>
+      <c r="U112" s="6">
         <v>0.63</v>
       </c>
-      <c r="U112" s="15" t="s">
+      <c r="V112" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="V112">
+      <c r="W112">
         <v>309</v>
       </c>
     </row>
-    <row r="113" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7295,24 +7756,24 @@
         <v>1</v>
       </c>
       <c r="O113">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>973</v>
       </c>
       <c r="Q113" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CD</v>
       </c>
-      <c r="T113" s="5">
+      <c r="U113" s="5">
         <v>0.67</v>
       </c>
-      <c r="U113" s="15" t="s">
+      <c r="V113" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="V113">
+      <c r="W113">
         <v>312</v>
       </c>
     </row>
-    <row r="114" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7353,24 +7814,32 @@
         <v>1</v>
       </c>
       <c r="O114">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>973</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CD</v>
       </c>
-      <c r="T114" s="5">
+      <c r="R114" t="str">
+        <f t="shared" ref="R114" si="115">Q114</f>
+        <v>03CD</v>
+      </c>
+      <c r="S114" t="str">
+        <f t="shared" ref="S114" si="116">"0x"&amp;R114</f>
+        <v>0x03CD</v>
+      </c>
+      <c r="U114" s="5">
         <v>0.71</v>
       </c>
-      <c r="U114" s="15" t="s">
+      <c r="V114" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="V114">
+      <c r="W114">
         <v>315</v>
       </c>
     </row>
-    <row r="115" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7411,24 +7880,24 @@
         <v>1</v>
       </c>
       <c r="O115">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>973</v>
       </c>
       <c r="Q115" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>03CD</v>
       </c>
-      <c r="T115" s="5">
+      <c r="U115" s="5">
         <v>0.74</v>
       </c>
-      <c r="U115" s="15" t="s">
+      <c r="V115" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="V115">
+      <c r="W115">
         <v>318</v>
       </c>
     </row>
-    <row r="116" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7469,24 +7938,32 @@
         <v>1</v>
       </c>
       <c r="O116">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>717</v>
       </c>
       <c r="Q116" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02CD</v>
       </c>
-      <c r="T116" s="5">
+      <c r="R116" t="str">
+        <f t="shared" ref="R116" si="117">Q116</f>
+        <v>02CD</v>
+      </c>
+      <c r="S116" t="str">
+        <f t="shared" ref="S116" si="118">"0x"&amp;R116</f>
+        <v>0x02CD</v>
+      </c>
+      <c r="U116" s="5">
         <v>0.77</v>
       </c>
-      <c r="U116" s="16" t="s">
+      <c r="V116" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="V116">
+      <c r="W116">
         <v>321</v>
       </c>
     </row>
-    <row r="117" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7527,24 +8004,24 @@
         <v>1</v>
       </c>
       <c r="O117">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>721</v>
       </c>
       <c r="Q117" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D1</v>
       </c>
-      <c r="T117" s="4">
+      <c r="U117" s="4">
         <v>0.8</v>
       </c>
-      <c r="U117" s="16" t="s">
+      <c r="V117" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="V117">
+      <c r="W117">
         <v>323</v>
       </c>
     </row>
-    <row r="118" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7585,24 +8062,32 @@
         <v>1</v>
       </c>
       <c r="O118">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>721</v>
       </c>
       <c r="Q118" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D1</v>
       </c>
-      <c r="T118" s="4">
+      <c r="R118" t="str">
+        <f t="shared" ref="R118" si="119">Q118</f>
+        <v>02D1</v>
+      </c>
+      <c r="S118" t="str">
+        <f t="shared" ref="S118" si="120">"0x"&amp;R118</f>
+        <v>0x02D1</v>
+      </c>
+      <c r="U118" s="4">
         <v>0.83</v>
       </c>
-      <c r="U118" s="16" t="s">
+      <c r="V118" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="V118">
+      <c r="W118">
         <v>326</v>
       </c>
     </row>
-    <row r="119" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -7643,24 +8128,24 @@
         <v>1</v>
       </c>
       <c r="O119">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>721</v>
       </c>
       <c r="Q119" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>02D1</v>
       </c>
-      <c r="T119" s="4">
+      <c r="U119" s="4">
         <v>0.86</v>
       </c>
-      <c r="U119" s="16" t="s">
+      <c r="V119" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="V119">
+      <c r="W119">
         <v>329</v>
       </c>
     </row>
-    <row r="120" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7701,24 +8186,32 @@
         <v>1</v>
       </c>
       <c r="O120">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>465</v>
       </c>
       <c r="Q120" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D1</v>
       </c>
-      <c r="T120" s="4">
+      <c r="R120" t="str">
+        <f t="shared" ref="R120" si="121">Q120</f>
+        <v>01D1</v>
+      </c>
+      <c r="S120" t="str">
+        <f t="shared" ref="S120" si="122">"0x"&amp;R120</f>
+        <v>0x01D1</v>
+      </c>
+      <c r="U120" s="4">
         <v>0.88</v>
       </c>
-      <c r="U120" s="17" t="s">
+      <c r="V120" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="V120">
+      <c r="W120">
         <v>332</v>
       </c>
     </row>
-    <row r="121" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7759,24 +8252,24 @@
         <v>1</v>
       </c>
       <c r="O121">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>469</v>
       </c>
       <c r="Q121" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D5</v>
       </c>
-      <c r="T121" s="7">
+      <c r="U121" s="7">
         <v>0.9</v>
       </c>
-      <c r="U121" s="17" t="s">
+      <c r="V121" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="V121">
+      <c r="W121">
         <v>335</v>
       </c>
     </row>
-    <row r="122" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7817,24 +8310,32 @@
         <v>1</v>
       </c>
       <c r="O122">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>469</v>
       </c>
       <c r="Q122" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D5</v>
       </c>
-      <c r="T122" s="7">
+      <c r="R122" t="str">
+        <f t="shared" ref="R122" si="123">Q122</f>
+        <v>01D5</v>
+      </c>
+      <c r="S122" t="str">
+        <f t="shared" ref="S122" si="124">"0x"&amp;R122</f>
+        <v>0x01D5</v>
+      </c>
+      <c r="U122" s="7">
         <v>0.92</v>
       </c>
-      <c r="U122" s="17" t="s">
+      <c r="V122" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="V122">
+      <c r="W122">
         <v>338</v>
       </c>
     </row>
-    <row r="123" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7875,24 +8376,24 @@
         <v>1</v>
       </c>
       <c r="O123">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>469</v>
       </c>
       <c r="Q123" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>01D5</v>
       </c>
-      <c r="T123" s="7">
+      <c r="U123" s="7">
         <v>0.94</v>
       </c>
-      <c r="U123" s="17" t="s">
+      <c r="V123" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="V123">
+      <c r="W123">
         <v>340</v>
       </c>
     </row>
-    <row r="124" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7933,24 +8434,32 @@
         <v>1</v>
       </c>
       <c r="O124">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>213</v>
       </c>
       <c r="Q124" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00D5</v>
       </c>
-      <c r="T124" s="7">
+      <c r="R124" t="str">
+        <f t="shared" ref="R124" si="125">Q124</f>
+        <v>00D5</v>
+      </c>
+      <c r="S124" t="str">
+        <f t="shared" ref="S124" si="126">"0x"&amp;R124</f>
+        <v>0x00D5</v>
+      </c>
+      <c r="U124" s="7">
         <v>0.96</v>
       </c>
-      <c r="U124" s="18" t="s">
+      <c r="V124" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="V124">
+      <c r="W124">
         <v>343</v>
       </c>
     </row>
-    <row r="125" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7991,24 +8500,24 @@
         <v>1</v>
       </c>
       <c r="O125">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>217</v>
       </c>
       <c r="Q125" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00D9</v>
       </c>
-      <c r="T125" s="8">
+      <c r="U125" s="8">
         <v>0.97</v>
       </c>
-      <c r="U125" s="18" t="s">
+      <c r="V125" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="V125">
+      <c r="W125">
         <v>346</v>
       </c>
     </row>
-    <row r="126" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -8049,24 +8558,32 @@
         <v>1</v>
       </c>
       <c r="O126">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>217</v>
       </c>
       <c r="Q126" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00D9</v>
       </c>
-      <c r="T126" s="8">
+      <c r="R126" t="str">
+        <f t="shared" ref="R126" si="127">Q126</f>
+        <v>00D9</v>
+      </c>
+      <c r="S126" t="str">
+        <f t="shared" ref="S126" si="128">"0x"&amp;R126</f>
+        <v>0x00D9</v>
+      </c>
+      <c r="U126" s="8">
         <v>0.98</v>
       </c>
-      <c r="U126" s="18" t="s">
+      <c r="V126" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="V126">
+      <c r="W126">
         <v>349</v>
       </c>
     </row>
-    <row r="127" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -8107,24 +8624,24 @@
         <v>1</v>
       </c>
       <c r="O127">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>217</v>
       </c>
       <c r="Q127" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>00D9</v>
       </c>
-      <c r="T127" s="8">
+      <c r="U127" s="8">
         <v>0.99</v>
       </c>
-      <c r="U127" s="18" t="s">
+      <c r="V127" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="V127">
+      <c r="W127">
         <v>352</v>
       </c>
     </row>
-    <row r="128" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -8165,24 +8682,32 @@
         <v>1</v>
       </c>
       <c r="O128">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>153</v>
       </c>
       <c r="Q128" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>0099</v>
       </c>
-      <c r="T128" s="8">
-        <v>1</v>
-      </c>
-      <c r="U128" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="V128">
+      <c r="R128" t="str">
+        <f t="shared" ref="R128" si="129">Q128</f>
+        <v>0099</v>
+      </c>
+      <c r="S128" t="str">
+        <f t="shared" ref="S128" si="130">"0x"&amp;R128</f>
+        <v>0x0099</v>
+      </c>
+      <c r="U128" s="8">
+        <v>1</v>
+      </c>
+      <c r="V128" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="W128">
         <v>354</v>
       </c>
     </row>
-    <row r="129" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -8223,20 +8748,20 @@
         <v>1</v>
       </c>
       <c r="O129">
-        <f t="shared" si="4"/>
+        <f t="shared" si="76"/>
         <v>157</v>
       </c>
       <c r="Q129" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="67"/>
         <v>009D</v>
       </c>
-      <c r="T129" s="10">
-        <v>1</v>
-      </c>
-      <c r="U129" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="V129">
+      <c r="U129" s="10">
+        <v>1</v>
+      </c>
+      <c r="V129" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="W129">
         <v>357</v>
       </c>
     </row>

</xml_diff>